<commit_message>
final experiment setup spreadsheet updated
</commit_message>
<xml_diff>
--- a/sampling/hyperparameter_setups.xlsx
+++ b/sampling/hyperparameter_setups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hank/Desktop/git_local/CSCI699-HW1/sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B6988F-43F4-D145-AFAB-A9C8E3C67118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5178B69C-DF7A-154B-A59A-E75E80374320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-1840" windowWidth="38400" windowHeight="21600" xr2:uid="{D357DB67-E97F-414D-9593-4AB2E677583C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
   <si>
     <t>HMC</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>[500, 2000]</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Hank</t>
   </si>
 </sst>
 </file>
@@ -148,12 +157,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -194,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -217,21 +244,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1C2A11-039E-714F-84D7-B613C7FF4261}">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,14 +642,14 @@
         <v>8</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
@@ -589,16 +661,16 @@
       <c r="D3" s="9">
         <v>40</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="21">
         <v>40</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="18" t="s">
         <v>16</v>
       </c>
     </row>
@@ -610,157 +682,184 @@
       <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="21">
         <v>1</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="7"/>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="9">
         <v>10000</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="21">
         <v>10000</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="18">
         <v>10000</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="2:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D8" s="21">
         <v>2</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F8" s="18">
         <v>2</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H8" s="21">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="12" t="s">
+    <row r="9" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B9" s="7"/>
+      <c r="C9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H9" s="21" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="7"/>
+      <c r="C11" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D11" s="21">
         <v>128</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E11" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F11" s="18">
         <v>128</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G11" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H11" s="21">
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
-      <c r="C11" s="12" t="s">
+    <row r="12" spans="2:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="B12" s="7"/>
+      <c r="C12" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E12" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="G12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H12" s="21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="14"/>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="11"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="15"/>
+      <c r="H16" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="30"/>
+      <c r="H17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="31"/>
+      <c r="H18" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -768,7 +867,7 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B8:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
HW3 roberta code updated
</commit_message>
<xml_diff>
--- a/sampling/hyperparameter_setups.xlsx
+++ b/sampling/hyperparameter_setups.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hank/Desktop/git_local/CSCI699-HW1/sampling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C7B673-3F0D-1443-9973-00AF7BD11DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958F453B-BFFE-F84C-900A-76377459DAC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35740" yWindow="-980" windowWidth="28800" windowHeight="16160" xr2:uid="{D357DB67-E97F-414D-9593-4AB2E677583C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{D357DB67-E97F-414D-9593-4AB2E677583C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
   <si>
     <t>HMC</t>
   </si>
@@ -85,48 +85,73 @@
     <t>data3: zebra</t>
   </si>
   <si>
+    <t>[500, 2000]</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Hank</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">[10, </t>
+      <t>[</t>
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2000</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>40</t>
+      <t>, 20000, 100000]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">[10, 40, </t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, 100]</t>
+      <t>]</t>
     </r>
-  </si>
-  <si>
-    <t>[500, 2000]</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>Hassan</t>
-  </si>
-  <si>
-    <t>Hank</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -148,6 +173,26 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -214,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -247,15 +292,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -268,15 +304,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -285,10 +312,25 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -614,7 +656,7 @@
   <dimension ref="B2:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -631,21 +673,21 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="5"/>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="28" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="29" t="s">
+      <c r="F2" s="27"/>
+      <c r="G2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="29"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -654,58 +696,58 @@
       <c r="D3" s="7">
         <v>40</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="15">
         <v>40</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="15" t="s">
-        <v>16</v>
+      <c r="H3" s="23" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="31"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="15">
         <v>1</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="31"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="7">
         <v>10000</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="15">
         <v>10000</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="23">
         <v>10000</v>
       </c>
     </row>
@@ -727,109 +769,109 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="2:8" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="15">
         <v>2</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="23">
         <v>2</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B9" s="31"/>
-      <c r="C9" s="17" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="31"/>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="14" t="s">
+      <c r="D10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="19" t="s">
+      <c r="F10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="18" t="s">
-        <v>17</v>
+      <c r="H10" s="15" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="31"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="15">
         <v>128</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="23">
         <v>128</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="15">
         <v>128</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B12" s="31"/>
-      <c r="C12" s="17" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="20" t="s">
+      <c r="F12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="15" t="s">
         <v>13</v>
       </c>
     </row>
@@ -839,19 +881,19 @@
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="G16" s="13"/>
       <c r="H16" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="20"/>
+      <c r="H17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G17" s="26"/>
-      <c r="H17" s="4" t="s">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="21"/>
+      <c r="H18" s="4" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G18" s="27"/>
-      <c r="H18" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>